<commit_message>
finished making ExcelReader tests
made all ExcelReader tests pass

fixed ExcelReader.GetTimeSeries to get proper path

added some excel test files
</commit_message>
<xml_diff>
--- a/DSSExcelTests/test-files/small-ir-ts.xlsx
+++ b/DSSExcelTests/test-files/small-ir-ts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DSSExcelPlugin\DSSExcelTests\test-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC45D3B9-4762-4ACD-A005-024984A71FDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0531F5CD-7B4D-47C7-9D9E-D03F3062FF0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13980" yWindow="4830" windowWidth="15330" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="405" windowWidth="15330" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>A</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>INST-VAL</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -393,16 +402,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -483,22 +493,22 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" s="2">
-        <v>43982.958333333336</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0</v>
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="2">
-        <v>43982.96875</v>
+        <v>43982.958333333336</v>
       </c>
       <c r="C9" s="3">
         <v>0</v>
@@ -506,10 +516,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" s="2">
-        <v>43982.979166666664</v>
+        <v>43982.96875</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
@@ -517,10 +527,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" s="2">
-        <v>43982.989583333336</v>
+        <v>43982.979166666664</v>
       </c>
       <c r="C11" s="3">
         <v>0</v>
@@ -528,10 +538,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="2">
-        <v>43983</v>
+        <v>43982.989583333336</v>
       </c>
       <c r="C12" s="3">
         <v>0</v>
@@ -539,10 +549,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2">
-        <v>43983.010416666664</v>
+        <v>43983</v>
       </c>
       <c r="C13" s="3">
         <v>0</v>
@@ -550,10 +560,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="2">
-        <v>43983.15625</v>
+        <v>43983.010416666664</v>
       </c>
       <c r="C14" s="3">
         <v>0</v>
@@ -561,10 +571,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="2">
-        <v>43983.166666666664</v>
+        <v>43983.020833333336</v>
       </c>
       <c r="C15" s="3">
         <v>0</v>
@@ -572,10 +582,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="2">
-        <v>43983.177083333336</v>
+        <v>43983.03125</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
@@ -583,12 +593,23 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2">
+        <v>43983.041666666664</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>10</v>
       </c>
-      <c r="B17" s="2">
-        <v>43983.1875</v>
-      </c>
-      <c r="C17" s="3">
+      <c r="B18" s="2">
+        <v>43983.197916666664</v>
+      </c>
+      <c r="C18" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>